<commit_message>
reorganization of some functions and analysis of the reaction time / single trial responses
</commit_message>
<xml_diff>
--- a/formant_analysis/PD_formant_freqs.xlsx
+++ b/formant_analysis/PD_formant_freqs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="620" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="520" windowWidth="21180" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="FCR" sheetId="2" r:id="rId1"/>
@@ -1353,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20494,13 +20494,24 @@
     <sortCondition ref="QY5:QY22"/>
   </sortState>
   <mergeCells count="37">
-    <mergeCell ref="QZ1:RI1"/>
-    <mergeCell ref="NZ1:OI1"/>
-    <mergeCell ref="OM1:OV1"/>
-    <mergeCell ref="OZ1:PI1"/>
-    <mergeCell ref="PM1:PV1"/>
-    <mergeCell ref="PZ1:QI1"/>
-    <mergeCell ref="QM1:QV1"/>
+    <mergeCell ref="BM1:BV1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="AN1:AV1"/>
+    <mergeCell ref="AZ1:BI1"/>
+    <mergeCell ref="HM1:HV1"/>
+    <mergeCell ref="BZ1:CI1"/>
+    <mergeCell ref="CM1:CV1"/>
+    <mergeCell ref="CZ1:DI1"/>
+    <mergeCell ref="DM1:DV1"/>
+    <mergeCell ref="DZ1:EI1"/>
+    <mergeCell ref="EM1:EV1"/>
+    <mergeCell ref="EZ1:FI1"/>
+    <mergeCell ref="FM1:FV1"/>
+    <mergeCell ref="FZ1:GI1"/>
+    <mergeCell ref="GM1:GV1"/>
+    <mergeCell ref="GZ1:HI1"/>
     <mergeCell ref="NM1:NV1"/>
     <mergeCell ref="HZ1:II1"/>
     <mergeCell ref="IM1:IV1"/>
@@ -20513,24 +20524,13 @@
     <mergeCell ref="LZ1:MI1"/>
     <mergeCell ref="MM1:MV1"/>
     <mergeCell ref="MZ1:NI1"/>
-    <mergeCell ref="HM1:HV1"/>
-    <mergeCell ref="BZ1:CI1"/>
-    <mergeCell ref="CM1:CV1"/>
-    <mergeCell ref="CZ1:DI1"/>
-    <mergeCell ref="DM1:DV1"/>
-    <mergeCell ref="DZ1:EI1"/>
-    <mergeCell ref="EM1:EV1"/>
-    <mergeCell ref="EZ1:FI1"/>
-    <mergeCell ref="FM1:FV1"/>
-    <mergeCell ref="FZ1:GI1"/>
-    <mergeCell ref="GM1:GV1"/>
-    <mergeCell ref="GZ1:HI1"/>
-    <mergeCell ref="BM1:BV1"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="P1:X1"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="AN1:AV1"/>
-    <mergeCell ref="AZ1:BI1"/>
+    <mergeCell ref="QZ1:RI1"/>
+    <mergeCell ref="NZ1:OI1"/>
+    <mergeCell ref="OM1:OV1"/>
+    <mergeCell ref="OZ1:PI1"/>
+    <mergeCell ref="PM1:PV1"/>
+    <mergeCell ref="PZ1:QI1"/>
+    <mergeCell ref="QM1:QV1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>